<commit_message>
Updated product backlog and release and sprint plan
</commit_message>
<xml_diff>
--- a/doc/User_Stories_Release_and_Sprint_Plans_Criteria/Product_Backlog.xlsx
+++ b/doc/User_Stories_Release_and_Sprint_Plans_Criteria/Product_Backlog.xlsx
@@ -1519,6 +1519,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2262,10 +2265,10 @@
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.5" footer="0.25"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId29"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId29"/>
+  <drawing r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>